<commit_message>
Finished pi wing hub project, added final features and exported manufacturing files.
</commit_message>
<xml_diff>
--- a/Builds/LAPARO/Hardware/PCB/Component Order 11192018.xlsx
+++ b/Builds/LAPARO/Hardware/PCB/Component Order 11192018.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Component</t>
   </si>
@@ -125,6 +125,21 @@
   </si>
   <si>
     <t>Straight, male headers</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Kingbright/WP710A10ID5V?qs=%2fha2pyFaduif%252bBBlxM5YV3XngdZOqN%252baoHyOgkHr2ji%2f1CmgLsWlCA%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/?qs=jBF9H7RTBaQ2jkR1uoa79Q%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Kingbright/WP710A10YD5V?qs=%2fha2pyFaduiSDnyyF%252bbBg%252budm3UQjOD8Q16lrjG8DUYITtew2gLhUg%3d%3d</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>5V, 3 mm</t>
   </si>
 </sst>
 </file>
@@ -546,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD941"/>
+  <dimension ref="A1:AD945"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F6" sqref="F6:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -653,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="K2" s="10">
-        <f t="shared" ref="K2:K5" si="0">I2*J2</f>
+        <f t="shared" ref="K2:K8" si="0">I2*J2</f>
         <v>19.98</v>
       </c>
       <c r="L2" s="1"/>
@@ -821,14 +836,27 @@
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="G6" s="17"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
+      <c r="H6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="0"/>
+        <v>10.35</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="9"/>
       <c r="N6" s="1"/>
@@ -853,18 +881,26 @@
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="D7" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="G7" s="17"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3" t="s">
-        <v>14</v>
+      <c r="H7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J7" s="3">
+        <v>25</v>
       </c>
       <c r="K7" s="2">
-        <f>SUM(K2:K6)</f>
-        <v>65.77</v>
+        <f t="shared" si="0"/>
+        <v>10.35</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="9"/>
@@ -890,14 +926,27 @@
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="F8" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="17"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
+      <c r="H8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J8" s="3">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>10.35</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="9"/>
       <c r="N8" s="1"/>
@@ -926,7 +975,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="15"/>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
@@ -958,7 +1007,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
@@ -992,8 +1041,13 @@
       <c r="G11" s="17"/>
       <c r="H11" s="1"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2">
+        <f>SUM(K2:K8)</f>
+        <v>96.819999999999979</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="9"/>
       <c r="N11" s="1"/>
@@ -1015,13 +1069,13 @@
       <c r="AD11" s="1"/>
     </row>
     <row r="12" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1047,13 +1101,13 @@
       <c r="AD12" s="1"/>
     </row>
     <row r="13" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
@@ -1079,13 +1133,13 @@
       <c r="AD13" s="1"/>
     </row>
     <row r="14" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="1"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
@@ -1111,13 +1165,13 @@
       <c r="AD14" s="1"/>
     </row>
     <row r="15" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="1"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
@@ -30774,11 +30828,142 @@
       <c r="AC941" s="1"/>
       <c r="AD941" s="1"/>
     </row>
+    <row r="942" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A942" s="2"/>
+      <c r="B942" s="2"/>
+      <c r="C942" s="2"/>
+      <c r="D942" s="1"/>
+      <c r="E942" s="1"/>
+      <c r="F942" s="1"/>
+      <c r="G942" s="1"/>
+      <c r="H942" s="1"/>
+      <c r="I942" s="2"/>
+      <c r="J942" s="3"/>
+      <c r="K942" s="2"/>
+      <c r="L942" s="1"/>
+      <c r="M942" s="9"/>
+      <c r="N942" s="1"/>
+      <c r="O942" s="1"/>
+      <c r="P942" s="1"/>
+      <c r="Q942" s="1"/>
+      <c r="R942" s="1"/>
+      <c r="S942" s="1"/>
+      <c r="T942" s="1"/>
+      <c r="U942" s="1"/>
+      <c r="V942" s="1"/>
+      <c r="W942" s="1"/>
+      <c r="X942" s="1"/>
+      <c r="Y942" s="1"/>
+      <c r="Z942" s="1"/>
+      <c r="AA942" s="1"/>
+      <c r="AB942" s="1"/>
+      <c r="AC942" s="1"/>
+      <c r="AD942" s="1"/>
+    </row>
+    <row r="943" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A943" s="2"/>
+      <c r="B943" s="2"/>
+      <c r="C943" s="2"/>
+      <c r="D943" s="1"/>
+      <c r="E943" s="1"/>
+      <c r="F943" s="1"/>
+      <c r="G943" s="1"/>
+      <c r="H943" s="1"/>
+      <c r="I943" s="2"/>
+      <c r="J943" s="3"/>
+      <c r="K943" s="2"/>
+      <c r="L943" s="1"/>
+      <c r="M943" s="9"/>
+      <c r="N943" s="1"/>
+      <c r="O943" s="1"/>
+      <c r="P943" s="1"/>
+      <c r="Q943" s="1"/>
+      <c r="R943" s="1"/>
+      <c r="S943" s="1"/>
+      <c r="T943" s="1"/>
+      <c r="U943" s="1"/>
+      <c r="V943" s="1"/>
+      <c r="W943" s="1"/>
+      <c r="X943" s="1"/>
+      <c r="Y943" s="1"/>
+      <c r="Z943" s="1"/>
+      <c r="AA943" s="1"/>
+      <c r="AB943" s="1"/>
+      <c r="AC943" s="1"/>
+      <c r="AD943" s="1"/>
+    </row>
+    <row r="944" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A944" s="2"/>
+      <c r="B944" s="2"/>
+      <c r="C944" s="2"/>
+      <c r="D944" s="1"/>
+      <c r="E944" s="1"/>
+      <c r="F944" s="1"/>
+      <c r="G944" s="1"/>
+      <c r="H944" s="1"/>
+      <c r="I944" s="2"/>
+      <c r="J944" s="3"/>
+      <c r="K944" s="2"/>
+      <c r="L944" s="1"/>
+      <c r="M944" s="9"/>
+      <c r="N944" s="1"/>
+      <c r="O944" s="1"/>
+      <c r="P944" s="1"/>
+      <c r="Q944" s="1"/>
+      <c r="R944" s="1"/>
+      <c r="S944" s="1"/>
+      <c r="T944" s="1"/>
+      <c r="U944" s="1"/>
+      <c r="V944" s="1"/>
+      <c r="W944" s="1"/>
+      <c r="X944" s="1"/>
+      <c r="Y944" s="1"/>
+      <c r="Z944" s="1"/>
+      <c r="AA944" s="1"/>
+      <c r="AB944" s="1"/>
+      <c r="AC944" s="1"/>
+      <c r="AD944" s="1"/>
+    </row>
+    <row r="945" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A945" s="2"/>
+      <c r="B945" s="2"/>
+      <c r="C945" s="2"/>
+      <c r="D945" s="1"/>
+      <c r="E945" s="1"/>
+      <c r="F945" s="1"/>
+      <c r="G945" s="1"/>
+      <c r="H945" s="1"/>
+      <c r="I945" s="2"/>
+      <c r="J945" s="3"/>
+      <c r="K945" s="2"/>
+      <c r="L945" s="1"/>
+      <c r="M945" s="9"/>
+      <c r="N945" s="1"/>
+      <c r="O945" s="1"/>
+      <c r="P945" s="1"/>
+      <c r="Q945" s="1"/>
+      <c r="R945" s="1"/>
+      <c r="S945" s="1"/>
+      <c r="T945" s="1"/>
+      <c r="U945" s="1"/>
+      <c r="V945" s="1"/>
+      <c r="W945" s="1"/>
+      <c r="X945" s="1"/>
+      <c r="Y945" s="1"/>
+      <c r="Z945" s="1"/>
+      <c r="AA945" s="1"/>
+      <c r="AB945" s="1"/>
+      <c r="AC945" s="1"/>
+      <c r="AD945" s="1"/>
+    </row>
   </sheetData>
   <sortState ref="A2:AD975">
     <sortCondition ref="B2:B975"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>